<commit_message>
Finalized recalibration (none needed)
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\CIS Updates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF5A23F8-C602-40B1-A543-652DDDE1A400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0D691F-AD47-4BD8-8C73-5AEA8AAB5AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="348" windowWidth="7500" windowHeight="6000" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
+    <workbookView xWindow="2928" yWindow="2988" windowWidth="12948" windowHeight="7944" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
   </bookViews>
   <sheets>
     <sheet name="August 2022" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Drawer</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>7/26</t>
+  </si>
+  <si>
+    <t>MASKED</t>
+  </si>
+  <si>
+    <t>LBA10</t>
+  </si>
+  <si>
+    <t>NOT IN UPDATE</t>
+  </si>
+  <si>
+    <t>7/21</t>
   </si>
 </sst>
 </file>
@@ -453,7 +465,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,7 +505,9 @@
       <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -510,16 +524,28 @@
       <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+    <row r="4" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>37</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -643,5 +669,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Crosschecked channels to recalibrate and flags to update
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0D691F-AD47-4BD8-8C73-5AEA8AAB5AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE9C457-5B60-4E4F-821C-3702E1E74477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2988" windowWidth="12948" windowHeight="7944" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
+    <workbookView xWindow="3276" yWindow="3336" windowWidth="12948" windowHeight="7944" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
   </bookViews>
   <sheets>
-    <sheet name="August 2022" sheetId="1" r:id="rId1"/>
+    <sheet name="September 2022" sheetId="2" r:id="rId1"/>
+    <sheet name="August 2022" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="63">
   <si>
     <t>Drawer</t>
   </si>
@@ -87,12 +88,162 @@
   <si>
     <t>7/21</t>
   </si>
+  <si>
+    <t>LBC24</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>8/22</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,6 +263,17 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -148,6 +310,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,11 +627,873 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1489683-C478-4051-88E8-BFE688253467}">
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="5"/>
+      <c r="B50" s="6"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F5A94A-A455-4BB9-9367-9D48260B09EE}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Presentation draft September, spreadsheets finalized
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE9C457-5B60-4E4F-821C-3702E1E74477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC27A8A-3513-475C-90F6-DE539F81BF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3276" yWindow="3336" windowWidth="12948" windowHeight="7944" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="67">
   <si>
     <t>Drawer</t>
   </si>
@@ -237,6 +237,18 @@
   </si>
   <si>
     <t>8/22</t>
+  </si>
+  <si>
+    <t>8/23</t>
+  </si>
+  <si>
+    <t>8/25</t>
+  </si>
+  <si>
+    <t>EBC46</t>
+  </si>
+  <si>
+    <t>LBC52</t>
   </si>
 </sst>
 </file>
@@ -296,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -314,6 +326,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,14 +646,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1489683-C478-4051-88E8-BFE688253467}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="8.88671875" style="6"/>
     <col min="6" max="6" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -643,7 +663,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -652,14 +672,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -673,11 +693,9 @@
       <c r="E2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -691,11 +709,9 @@
       <c r="E3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -709,11 +725,9 @@
       <c r="E4" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -726,11 +740,9 @@
       <c r="E5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -743,11 +755,9 @@
       <c r="E6" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -760,11 +770,9 @@
       <c r="E7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -777,11 +785,9 @@
       <c r="E8" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -794,11 +800,9 @@
       <c r="E9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -811,11 +815,9 @@
       <c r="E10" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -828,11 +830,9 @@
       <c r="E11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
@@ -845,11 +845,9 @@
       <c r="E12" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -862,11 +860,9 @@
       <c r="E13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -879,11 +875,9 @@
       <c r="E14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -896,11 +890,9 @@
       <c r="E15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -913,11 +905,9 @@
       <c r="E16" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -930,11 +920,9 @@
       <c r="E17" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>13</v>
       </c>
@@ -947,11 +935,9 @@
       <c r="E18" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -964,11 +950,9 @@
       <c r="E19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>13</v>
       </c>
@@ -981,11 +965,9 @@
       <c r="E20" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -998,11 +980,9 @@
       <c r="E21" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>13</v>
       </c>
@@ -1015,11 +995,9 @@
       <c r="E22" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -1032,11 +1010,9 @@
       <c r="E23" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
@@ -1049,11 +1025,9 @@
       <c r="E24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -1066,11 +1040,9 @@
       <c r="E25" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
@@ -1083,11 +1055,9 @@
       <c r="E26" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -1100,11 +1070,9 @@
       <c r="E27" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>13</v>
       </c>
@@ -1117,11 +1085,9 @@
       <c r="E28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -1134,11 +1100,9 @@
       <c r="E29" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F29" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
@@ -1151,11 +1115,9 @@
       <c r="E30" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
@@ -1168,11 +1130,9 @@
       <c r="E31" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>13</v>
       </c>
@@ -1185,11 +1145,9 @@
       <c r="E32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>13</v>
       </c>
@@ -1202,11 +1160,9 @@
       <c r="E33" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>13</v>
       </c>
@@ -1219,11 +1175,9 @@
       <c r="E34" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
@@ -1236,11 +1190,9 @@
       <c r="E35" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>13</v>
       </c>
@@ -1253,11 +1205,9 @@
       <c r="E36" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>13</v>
       </c>
@@ -1270,11 +1220,9 @@
       <c r="E37" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>13</v>
       </c>
@@ -1287,11 +1235,9 @@
       <c r="E38" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>13</v>
       </c>
@@ -1304,11 +1250,9 @@
       <c r="E39" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>13</v>
       </c>
@@ -1321,11 +1265,9 @@
       <c r="E40" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>13</v>
       </c>
@@ -1338,11 +1280,9 @@
       <c r="E41" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>13</v>
       </c>
@@ -1355,11 +1295,9 @@
       <c r="E42" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
@@ -1372,11 +1310,9 @@
       <c r="E43" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>13</v>
       </c>
@@ -1389,11 +1325,9 @@
       <c r="E44" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>13</v>
       </c>
@@ -1406,11 +1340,9 @@
       <c r="E45" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>13</v>
       </c>
@@ -1423,11 +1355,9 @@
       <c r="E46" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F46" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>13</v>
       </c>
@@ -1440,11 +1370,9 @@
       <c r="E47" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>13</v>
       </c>
@@ -1457,11 +1385,9 @@
       <c r="E48" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>13</v>
       </c>
@@ -1474,17 +1400,783 @@
       <c r="E49" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="5"/>
-      <c r="B50" s="6"/>
+      <c r="A50" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="7">
+        <v>0</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="7">
+        <v>0</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="7">
+        <v>0</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="7">
+        <v>0</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="7">
+        <v>0</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="7">
+        <v>0</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="7">
+        <v>0</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="7">
+        <v>0</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" s="7">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="7">
+        <v>0</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="7">
+        <v>0</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="7">
+        <v>0</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="7">
+        <v>0</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="7">
+        <v>0</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" s="7">
+        <v>0</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66" s="7">
+        <v>0</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" s="7">
+        <v>0</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C68" s="7">
+        <v>0</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="7">
+        <v>0</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="7">
+        <v>0</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C71" s="7">
+        <v>0</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B72" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C72" s="7">
+        <v>0</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C73" s="7">
+        <v>0</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C74" s="7">
+        <v>0</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C75" s="7">
+        <v>0</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" s="7">
+        <v>0</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C77" s="7">
+        <v>0</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C78" s="7">
+        <v>0</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C79" s="7">
+        <v>0</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C80" s="7">
+        <v>0</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C81" s="7">
+        <v>0</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C82" s="7">
+        <v>0</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C83" s="7">
+        <v>0</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C84" s="7">
+        <v>0</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C85" s="7">
+        <v>0</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" s="7">
+        <v>0</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C87" s="7">
+        <v>0</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C88" s="7">
+        <v>0</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C89" s="7">
+        <v>0</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C90" s="7">
+        <v>0</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C91" s="7">
+        <v>0</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C92" s="7">
+        <v>0</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C93" s="7">
+        <v>0</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C94" s="7">
+        <v>0</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C95" s="7">
+        <v>0</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C96" s="7">
+        <v>0</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C97" s="7">
+        <v>0</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="7"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="5"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="7"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="5"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="7"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" s="5"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" s="7"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105" s="5"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106" s="7"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107" s="5"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108" s="7"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109" s="5"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110" s="7"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A111" s="5"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A112" s="7"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="5"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="7"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="5"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="7"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="5"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="7"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="5"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="7"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="5"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="7"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="5"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="7"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="5"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="7"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="5"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="7"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="5"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added flag changes and channels to recalibrate
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC27A8A-3513-475C-90F6-DE539F81BF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40750AB8-3A42-439E-B7C8-E18FE03ABA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3276" yWindow="3336" windowWidth="12948" windowHeight="7944" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
   </bookViews>
   <sheets>
-    <sheet name="September 2022" sheetId="2" r:id="rId1"/>
-    <sheet name="August 2022" sheetId="1" r:id="rId2"/>
+    <sheet name="October 2022" sheetId="3" r:id="rId1"/>
+    <sheet name="September 2022" sheetId="2" r:id="rId2"/>
+    <sheet name="August 2022" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="73">
   <si>
     <t>Drawer</t>
   </si>
@@ -249,6 +250,24 @@
   </si>
   <si>
     <t>LBC52</t>
+  </si>
+  <si>
+    <t>LBA03</t>
+  </si>
+  <si>
+    <t>LBA51</t>
+  </si>
+  <si>
+    <t>EBA61</t>
+  </si>
+  <si>
+    <t>9/26</t>
+  </si>
+  <si>
+    <t>9/22</t>
+  </si>
+  <si>
+    <t>9/8</t>
   </si>
 </sst>
 </file>
@@ -645,11 +664,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B6F8C3-E6AA-4F4A-B269-8A09BBE92021}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2">
+        <v>34</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1489683-C478-4051-88E8-BFE688253467}">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2180,7 +2308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F5A94A-A455-4BB9-9367-9D48260B09EE}">
   <dimension ref="A1:G17"/>
   <sheetViews>

</xml_diff>

<commit_message>
November realibrations and flags
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40750AB8-3A42-439E-B7C8-E18FE03ABA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A541599E-B72F-4A0B-8BE6-4C6D484AE18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
   </bookViews>
   <sheets>
-    <sheet name="October 2022" sheetId="3" r:id="rId1"/>
+    <sheet name="November 2022" sheetId="3" r:id="rId1"/>
     <sheet name="September 2022" sheetId="2" r:id="rId2"/>
     <sheet name="August 2022" sheetId="1" r:id="rId3"/>
   </sheets>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="70">
   <si>
     <t>Drawer</t>
   </si>
@@ -252,22 +252,13 @@
     <t>LBC52</t>
   </si>
   <si>
-    <t>LBA03</t>
-  </si>
-  <si>
     <t>LBA51</t>
   </si>
   <si>
-    <t>EBA61</t>
-  </si>
-  <si>
-    <t>9/26</t>
-  </si>
-  <si>
-    <t>9/22</t>
-  </si>
-  <si>
-    <t>9/8</t>
+    <t>10/13</t>
+  </si>
+  <si>
+    <t>LBC62</t>
   </si>
 </sst>
 </file>
@@ -665,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B6F8C3-E6AA-4F4A-B269-8A09BBE92021}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,72 +689,30 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B3">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
         <v>68</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recalibrations, flag changes, and notes file finalized
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A541599E-B72F-4A0B-8BE6-4C6D484AE18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7597A5C3-246A-4B69-80D4-80AEE2E97A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
   </bookViews>
   <sheets>
-    <sheet name="November 2022" sheetId="3" r:id="rId1"/>
-    <sheet name="September 2022" sheetId="2" r:id="rId2"/>
-    <sheet name="August 2022" sheetId="1" r:id="rId3"/>
+    <sheet name="February 2023" sheetId="4" r:id="rId1"/>
+    <sheet name="November 2022" sheetId="3" r:id="rId2"/>
+    <sheet name="September 2022" sheetId="2" r:id="rId3"/>
+    <sheet name="August 2022" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="80">
   <si>
     <t>Drawer</t>
   </si>
@@ -260,12 +261,42 @@
   <si>
     <t>LBC62</t>
   </si>
+  <si>
+    <t>EBA40</t>
+  </si>
+  <si>
+    <t>02/16</t>
+  </si>
+  <si>
+    <t>EBA61</t>
+  </si>
+  <si>
+    <t>02/16-02/23</t>
+  </si>
+  <si>
+    <t>EBC34</t>
+  </si>
+  <si>
+    <t>02/10</t>
+  </si>
+  <si>
+    <t>LBC17</t>
+  </si>
+  <si>
+    <t>LBC49</t>
+  </si>
+  <si>
+    <t>Not in update?</t>
+  </si>
+  <si>
+    <t>I do not undertstand this behaviour (will link plots)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +328,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -318,30 +356,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,10 +692,944 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060F0EBB-53EB-4156-B91F-26E5E9739AE6}">
+  <dimension ref="A1:F58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.44140625" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6">
+        <v>38</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7">
+        <v>39</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>40</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15">
+        <v>40</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18">
+        <v>41</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="8">
+        <v>15</v>
+      </c>
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="8">
+        <v>15</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21">
+        <v>30</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22">
+        <v>31</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25">
+        <v>36</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26">
+        <v>37</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28">
+        <v>31</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29">
+        <v>32</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31">
+        <v>36</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32">
+        <v>37</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39">
+        <v>24</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40">
+        <v>25</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41">
+        <v>26</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42">
+        <v>27</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43">
+        <v>28</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44">
+        <v>29</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45">
+        <v>33</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46">
+        <v>34</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47">
+        <v>35</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48">
+        <v>24</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>77</v>
+      </c>
+      <c r="B49">
+        <v>25</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50">
+        <v>26</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51">
+        <v>27</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52">
+        <v>28</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53">
+        <v>29</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54">
+        <v>33</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F54" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55">
+        <v>34</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56">
+        <v>35</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F56" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57">
+        <v>34</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58">
+        <v>34</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B6F8C3-E6AA-4F4A-B269-8A09BBE92021}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -671,7 +1642,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -680,7 +1651,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -721,7 +1692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1489683-C478-4051-88E8-BFE688253467}">
   <dimension ref="A1:F130"/>
   <sheetViews>
@@ -740,7 +1711,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -749,7 +1720,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1486,7 +2457,7 @@
       <c r="B50" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="2">
         <v>0</v>
       </c>
       <c r="E50" s="6" t="s">
@@ -1494,13 +2465,13 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="2">
         <v>0</v>
       </c>
       <c r="E51" s="6" t="s">
@@ -1514,7 +2485,7 @@
       <c r="B52" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="2">
         <v>0</v>
       </c>
       <c r="E52" s="6" t="s">
@@ -1522,13 +2493,13 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="2">
         <v>0</v>
       </c>
       <c r="E53" s="6" t="s">
@@ -1542,7 +2513,7 @@
       <c r="B54" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="2">
         <v>0</v>
       </c>
       <c r="E54" s="6" t="s">
@@ -1550,13 +2521,13 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C55" s="2">
         <v>0</v>
       </c>
       <c r="E55" s="6" t="s">
@@ -1570,7 +2541,7 @@
       <c r="B56" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="2">
         <v>0</v>
       </c>
       <c r="E56" s="6" t="s">
@@ -1578,13 +2549,13 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="2">
         <v>0</v>
       </c>
       <c r="E57" s="6" t="s">
@@ -1598,7 +2569,7 @@
       <c r="B58" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="2">
         <v>0</v>
       </c>
       <c r="E58" s="6" t="s">
@@ -1606,13 +2577,13 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="2">
         <v>0</v>
       </c>
       <c r="E59" s="6" t="s">
@@ -1626,7 +2597,7 @@
       <c r="B60" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="2">
         <v>0</v>
       </c>
       <c r="E60" s="6" t="s">
@@ -1634,13 +2605,13 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="7">
+      <c r="C61" s="2">
         <v>0</v>
       </c>
       <c r="E61" s="6" t="s">
@@ -1654,7 +2625,7 @@
       <c r="B62" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="2">
         <v>0</v>
       </c>
       <c r="E62" s="6" t="s">
@@ -1662,13 +2633,13 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="2">
         <v>0</v>
       </c>
       <c r="E63" s="6" t="s">
@@ -1682,7 +2653,7 @@
       <c r="B64" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="2">
         <v>0</v>
       </c>
       <c r="E64" s="6" t="s">
@@ -1690,13 +2661,13 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="2">
         <v>0</v>
       </c>
       <c r="E65" s="6" t="s">
@@ -1710,7 +2681,7 @@
       <c r="B66" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C66" s="7">
+      <c r="C66" s="2">
         <v>0</v>
       </c>
       <c r="E66" s="6" t="s">
@@ -1718,13 +2689,13 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="2">
         <v>0</v>
       </c>
       <c r="E67" s="6" t="s">
@@ -1738,7 +2709,7 @@
       <c r="B68" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="2">
         <v>0</v>
       </c>
       <c r="E68" s="6" t="s">
@@ -1752,7 +2723,7 @@
       <c r="B69" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="2">
         <v>0</v>
       </c>
       <c r="E69" s="6" t="s">
@@ -1760,13 +2731,13 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="2">
         <v>0</v>
       </c>
       <c r="E70" s="6" t="s">
@@ -1780,7 +2751,7 @@
       <c r="B71" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="2">
         <v>0</v>
       </c>
       <c r="E71" s="6" t="s">
@@ -1788,13 +2759,13 @@
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="2">
         <v>0</v>
       </c>
       <c r="E72" s="6" t="s">
@@ -1808,7 +2779,7 @@
       <c r="B73" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="2">
         <v>0</v>
       </c>
       <c r="E73" s="6" t="s">
@@ -1816,13 +2787,13 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="2">
         <v>0</v>
       </c>
       <c r="E74" s="6" t="s">
@@ -1836,7 +2807,7 @@
       <c r="B75" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="2">
         <v>0</v>
       </c>
       <c r="E75" s="6" t="s">
@@ -1844,13 +2815,13 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C76" s="7">
+      <c r="C76" s="2">
         <v>0</v>
       </c>
       <c r="E76" s="6" t="s">
@@ -1864,7 +2835,7 @@
       <c r="B77" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="2">
         <v>0</v>
       </c>
       <c r="E77" s="6" t="s">
@@ -1872,13 +2843,13 @@
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C78" s="2">
         <v>0</v>
       </c>
       <c r="E78" s="6" t="s">
@@ -1892,7 +2863,7 @@
       <c r="B79" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C79" s="7">
+      <c r="C79" s="2">
         <v>0</v>
       </c>
       <c r="E79" s="6" t="s">
@@ -1900,13 +2871,13 @@
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="2">
         <v>0</v>
       </c>
       <c r="E80" s="6" t="s">
@@ -1920,7 +2891,7 @@
       <c r="B81" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C81" s="7">
+      <c r="C81" s="2">
         <v>0</v>
       </c>
       <c r="E81" s="6" t="s">
@@ -1928,13 +2899,13 @@
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C82" s="7">
+      <c r="C82" s="2">
         <v>0</v>
       </c>
       <c r="E82" s="6" t="s">
@@ -1948,7 +2919,7 @@
       <c r="B83" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C83" s="7">
+      <c r="C83" s="2">
         <v>0</v>
       </c>
       <c r="E83" s="6" t="s">
@@ -1956,13 +2927,13 @@
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C84" s="7">
+      <c r="C84" s="2">
         <v>0</v>
       </c>
       <c r="E84" s="6" t="s">
@@ -1976,7 +2947,7 @@
       <c r="B85" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C85" s="7">
+      <c r="C85" s="2">
         <v>0</v>
       </c>
       <c r="E85" s="6" t="s">
@@ -1984,13 +2955,13 @@
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C86" s="7">
+      <c r="C86" s="2">
         <v>0</v>
       </c>
       <c r="E86" s="6" t="s">
@@ -2004,7 +2975,7 @@
       <c r="B87" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C87" s="7">
+      <c r="C87" s="2">
         <v>0</v>
       </c>
       <c r="E87" s="6" t="s">
@@ -2012,13 +2983,13 @@
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C88" s="7">
+      <c r="C88" s="2">
         <v>0</v>
       </c>
       <c r="E88" s="6" t="s">
@@ -2032,7 +3003,7 @@
       <c r="B89" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C89" s="7">
+      <c r="C89" s="2">
         <v>0</v>
       </c>
       <c r="E89" s="6" t="s">
@@ -2040,13 +3011,13 @@
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C90" s="7">
+      <c r="C90" s="2">
         <v>0</v>
       </c>
       <c r="E90" s="6" t="s">
@@ -2060,7 +3031,7 @@
       <c r="B91" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C91" s="7">
+      <c r="C91" s="2">
         <v>0</v>
       </c>
       <c r="E91" s="6" t="s">
@@ -2068,13 +3039,13 @@
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C92" s="7">
+      <c r="C92" s="2">
         <v>0</v>
       </c>
       <c r="E92" s="6" t="s">
@@ -2088,7 +3059,7 @@
       <c r="B93" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C93" s="7">
+      <c r="C93" s="2">
         <v>0</v>
       </c>
       <c r="E93" s="6" t="s">
@@ -2096,13 +3067,13 @@
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C94" s="7">
+      <c r="C94" s="2">
         <v>0</v>
       </c>
       <c r="E94" s="6" t="s">
@@ -2116,7 +3087,7 @@
       <c r="B95" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C95" s="7">
+      <c r="C95" s="2">
         <v>0</v>
       </c>
       <c r="E95" s="6" t="s">
@@ -2124,13 +3095,13 @@
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C96" s="7">
+      <c r="C96" s="2">
         <v>0</v>
       </c>
       <c r="E96" s="6" t="s">
@@ -2144,7 +3115,7 @@
       <c r="B97" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C97" s="7">
+      <c r="C97" s="2">
         <v>0</v>
       </c>
       <c r="E97" s="6" t="s">
@@ -2152,103 +3123,103 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" s="7"/>
+      <c r="A98" s="2"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="5"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A100" s="7"/>
+      <c r="A100" s="2"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="5"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" s="7"/>
+      <c r="A102" s="2"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="5"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="7"/>
+      <c r="A104" s="2"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="5"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" s="7"/>
+      <c r="A106" s="2"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="5"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" s="7"/>
+      <c r="A108" s="2"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="5"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" s="7"/>
+      <c r="A110" s="2"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="5"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="7"/>
+      <c r="A112" s="2"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" s="5"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" s="7"/>
+      <c r="A114" s="2"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" s="5"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" s="7"/>
+      <c r="A116" s="2"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" s="5"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" s="7"/>
+      <c r="A118" s="2"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" s="5"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" s="7"/>
+      <c r="A120" s="2"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" s="5"/>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" s="7"/>
+      <c r="A122" s="2"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" s="5"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" s="7"/>
+      <c r="A124" s="2"/>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" s="5"/>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" s="7"/>
+      <c r="A126" s="2"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" s="5"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" s="7"/>
+      <c r="A128" s="2"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="5"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" s="7"/>
+      <c r="A130" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2257,7 +3228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F5A94A-A455-4BB9-9367-9D48260B09EE}">
   <dimension ref="A1:G17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Flag and Recalibrations for March 2023
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7597A5C3-246A-4B69-80D4-80AEE2E97A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD7A094-F7DC-439B-8AB2-2A5D49D4EE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="15150" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
   </bookViews>
   <sheets>
-    <sheet name="February 2023" sheetId="4" r:id="rId1"/>
-    <sheet name="November 2022" sheetId="3" r:id="rId2"/>
-    <sheet name="September 2022" sheetId="2" r:id="rId3"/>
-    <sheet name="August 2022" sheetId="1" r:id="rId4"/>
+    <sheet name="March 2023" sheetId="5" r:id="rId1"/>
+    <sheet name="February 2023" sheetId="4" r:id="rId2"/>
+    <sheet name="November 2022" sheetId="3" r:id="rId3"/>
+    <sheet name="September 2022" sheetId="2" r:id="rId4"/>
+    <sheet name="August 2022" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="81">
   <si>
     <t>Drawer</t>
   </si>
@@ -290,6 +291,9 @@
   </si>
   <si>
     <t>I do not undertstand this behaviour (will link plots)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONE: ALL ARE BADCIS, SO THERE IS NO POINT IN RECALIBRATING THEM </t>
   </si>
 </sst>
 </file>
@@ -692,10 +696,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55F0D52-EB9A-4BE1-87C5-1462586BBE43}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.44140625" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="5:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060F0EBB-53EB-4156-B91F-26E5E9739AE6}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
@@ -1625,7 +1679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B6F8C3-E6AA-4F4A-B269-8A09BBE92021}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1692,7 +1746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1489683-C478-4051-88E8-BFE688253467}">
   <dimension ref="A1:F130"/>
   <sheetViews>
@@ -3228,7 +3282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F5A94A-A455-4BB9-9367-9D48260B09EE}">
   <dimension ref="A1:G17"/>
   <sheetViews>

</xml_diff>

<commit_message>
June 2023 flag changes, channels to recalibrate, and presentation
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Channels to Recalibrate.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD7A094-F7DC-439B-8AB2-2A5D49D4EE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AD5FB8-4482-4A71-B26C-9096FDFC5FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="15150" xr2:uid="{8F1C0F43-9C8B-4BF7-AC8D-7B3E8AE2C835}"/>
   </bookViews>
   <sheets>
-    <sheet name="March 2023" sheetId="5" r:id="rId1"/>
-    <sheet name="February 2023" sheetId="4" r:id="rId2"/>
-    <sheet name="November 2022" sheetId="3" r:id="rId3"/>
-    <sheet name="September 2022" sheetId="2" r:id="rId4"/>
-    <sheet name="August 2022" sheetId="1" r:id="rId5"/>
+    <sheet name="May 2023" sheetId="6" r:id="rId1"/>
+    <sheet name="March 2023" sheetId="5" r:id="rId2"/>
+    <sheet name="February 2023" sheetId="4" r:id="rId3"/>
+    <sheet name="November 2022" sheetId="3" r:id="rId4"/>
+    <sheet name="September 2022" sheetId="2" r:id="rId5"/>
+    <sheet name="August 2022" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="86">
   <si>
     <t>Drawer</t>
   </si>
@@ -294,6 +295,21 @@
   </si>
   <si>
     <t xml:space="preserve">NONE: ALL ARE BADCIS, SO THERE IS NO POINT IN RECALIBRATING THEM </t>
+  </si>
+  <si>
+    <t>EBA49</t>
+  </si>
+  <si>
+    <t>06/01</t>
+  </si>
+  <si>
+    <t>05/07</t>
+  </si>
+  <si>
+    <t>New Date (MM/DD)</t>
+  </si>
+  <si>
+    <t>LBA37</t>
   </si>
 </sst>
 </file>
@@ -696,19 +712,100 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA61E91D-6F29-40D0-A05E-9BBDFAC146AC}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" ht="39" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55F0D52-EB9A-4BE1-87C5-1462586BBE43}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,15 +825,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="5:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="5:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E20" s="9"/>
     </row>
   </sheetData>
@@ -745,20 +842,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060F0EBB-53EB-4156-B91F-26E5E9739AE6}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -778,7 +875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -792,7 +889,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -806,7 +903,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -820,7 +917,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -834,7 +931,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -851,7 +948,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -868,7 +965,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -885,7 +982,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -899,7 +996,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -913,7 +1010,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -927,7 +1024,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -944,7 +1041,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -961,7 +1058,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -975,7 +1072,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -992,7 +1089,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -1006,7 +1103,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -1023,7 +1120,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -1040,7 +1137,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
@@ -1057,7 +1154,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>72</v>
       </c>
@@ -1074,7 +1171,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1088,7 +1185,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1105,7 +1202,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -1122,7 +1219,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1139,7 +1236,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -1153,7 +1250,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -1170,7 +1267,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -1184,7 +1281,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -1201,7 +1298,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -1215,7 +1312,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1232,7 +1329,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -1249,7 +1346,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -1266,7 +1363,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -1283,7 +1380,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -1300,7 +1397,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -1317,7 +1414,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -1334,7 +1431,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>76</v>
       </c>
@@ -1351,7 +1448,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>76</v>
       </c>
@@ -1368,7 +1465,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>77</v>
       </c>
@@ -1385,7 +1482,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>77</v>
       </c>
@@ -1399,7 +1496,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1413,7 +1510,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -1427,7 +1524,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -1441,7 +1538,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -1455,7 +1552,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -1472,7 +1569,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>77</v>
       </c>
@@ -1489,7 +1586,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -1506,7 +1603,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -1520,7 +1617,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>77</v>
       </c>
@@ -1534,7 +1631,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -1551,7 +1648,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>77</v>
       </c>
@@ -1565,7 +1662,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>77</v>
       </c>
@@ -1579,7 +1676,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>77</v>
       </c>
@@ -1593,7 +1690,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>77</v>
       </c>
@@ -1610,7 +1707,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>77</v>
       </c>
@@ -1627,7 +1724,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>77</v>
       </c>
@@ -1644,7 +1741,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -1658,7 +1755,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -1679,7 +1776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B6F8C3-E6AA-4F4A-B269-8A09BBE92021}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1687,12 +1784,12 @@
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="8.88671875" style="6"/>
+    <col min="5" max="5" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1712,7 +1809,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1726,7 +1823,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -1746,7 +1843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1489683-C478-4051-88E8-BFE688253467}">
   <dimension ref="A1:F130"/>
   <sheetViews>
@@ -1754,14 +1851,14 @@
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="6"/>
-    <col min="5" max="5" width="8.88671875" style="6"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="6"/>
+    <col min="5" max="5" width="8.85546875" style="6"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1781,7 +1878,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
@@ -1797,7 +1894,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1813,7 +1910,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -1829,7 +1926,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -1844,7 +1941,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
@@ -1859,7 +1956,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1874,7 +1971,7 @@
       </c>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1889,7 +1986,7 @@
       </c>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1904,7 +2001,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1919,7 +2016,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -1934,7 +2031,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
@@ -1949,7 +2046,7 @@
       </c>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1964,7 +2061,7 @@
       </c>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
@@ -1979,7 +2076,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1994,7 +2091,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -2009,7 +2106,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2024,7 +2121,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>13</v>
       </c>
@@ -2039,7 +2136,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -2054,7 +2151,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>13</v>
       </c>
@@ -2069,7 +2166,7 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -2084,7 +2181,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>13</v>
       </c>
@@ -2099,7 +2196,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -2114,7 +2211,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
@@ -2129,7 +2226,7 @@
       </c>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
@@ -2144,7 +2241,7 @@
       </c>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>13</v>
       </c>
@@ -2159,7 +2256,7 @@
       </c>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -2174,7 +2271,7 @@
       </c>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>13</v>
       </c>
@@ -2189,7 +2286,7 @@
       </c>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>13</v>
       </c>
@@ -2204,7 +2301,7 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
@@ -2219,7 +2316,7 @@
       </c>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
@@ -2234,7 +2331,7 @@
       </c>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>13</v>
       </c>
@@ -2249,7 +2346,7 @@
       </c>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>13</v>
       </c>
@@ -2264,7 +2361,7 @@
       </c>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>13</v>
       </c>
@@ -2279,7 +2376,7 @@
       </c>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
@@ -2294,7 +2391,7 @@
       </c>
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>13</v>
       </c>
@@ -2309,7 +2406,7 @@
       </c>
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>13</v>
       </c>
@@ -2324,7 +2421,7 @@
       </c>
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>13</v>
       </c>
@@ -2339,7 +2436,7 @@
       </c>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>13</v>
       </c>
@@ -2354,7 +2451,7 @@
       </c>
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>13</v>
       </c>
@@ -2369,7 +2466,7 @@
       </c>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>13</v>
       </c>
@@ -2384,7 +2481,7 @@
       </c>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>13</v>
       </c>
@@ -2399,7 +2496,7 @@
       </c>
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
@@ -2414,7 +2511,7 @@
       </c>
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>13</v>
       </c>
@@ -2429,7 +2526,7 @@
       </c>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>13</v>
       </c>
@@ -2444,7 +2541,7 @@
       </c>
       <c r="F45" s="2"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>13</v>
       </c>
@@ -2459,7 +2556,7 @@
       </c>
       <c r="F46" s="2"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>13</v>
       </c>
@@ -2474,7 +2571,7 @@
       </c>
       <c r="F47" s="2"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>13</v>
       </c>
@@ -2489,7 +2586,7 @@
       </c>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>13</v>
       </c>
@@ -2504,7 +2601,7 @@
       </c>
       <c r="F49" s="2"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>65</v>
       </c>
@@ -2518,7 +2615,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>66</v>
       </c>
@@ -2532,7 +2629,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>66</v>
       </c>
@@ -2546,7 +2643,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>66</v>
       </c>
@@ -2560,7 +2657,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>66</v>
       </c>
@@ -2574,7 +2671,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
@@ -2588,7 +2685,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>66</v>
       </c>
@@ -2602,7 +2699,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>66</v>
       </c>
@@ -2616,7 +2713,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>66</v>
       </c>
@@ -2630,7 +2727,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
@@ -2644,7 +2741,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>66</v>
       </c>
@@ -2658,7 +2755,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
@@ -2672,7 +2769,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>66</v>
       </c>
@@ -2686,7 +2783,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>66</v>
       </c>
@@ -2700,7 +2797,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>66</v>
       </c>
@@ -2714,7 +2811,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>66</v>
       </c>
@@ -2728,7 +2825,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>66</v>
       </c>
@@ -2742,7 +2839,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
@@ -2756,7 +2853,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>66</v>
       </c>
@@ -2770,7 +2867,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>66</v>
       </c>
@@ -2784,7 +2881,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
@@ -2798,7 +2895,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>66</v>
       </c>
@@ -2812,7 +2909,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>66</v>
       </c>
@@ -2826,7 +2923,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>66</v>
       </c>
@@ -2840,7 +2937,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>66</v>
       </c>
@@ -2854,7 +2951,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>66</v>
       </c>
@@ -2868,7 +2965,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>66</v>
       </c>
@@ -2882,7 +2979,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>66</v>
       </c>
@@ -2896,7 +2993,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>66</v>
       </c>
@@ -2910,7 +3007,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>66</v>
       </c>
@@ -2924,7 +3021,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>66</v>
       </c>
@@ -2938,7 +3035,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>66</v>
       </c>
@@ -2952,7 +3049,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>66</v>
       </c>
@@ -2966,7 +3063,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>66</v>
       </c>
@@ -2980,7 +3077,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>66</v>
       </c>
@@ -2994,7 +3091,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>66</v>
       </c>
@@ -3008,7 +3105,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>66</v>
       </c>
@@ -3022,7 +3119,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>66</v>
       </c>
@@ -3036,7 +3133,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>66</v>
       </c>
@@ -3050,7 +3147,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>66</v>
       </c>
@@ -3064,7 +3161,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>66</v>
       </c>
@@ -3078,7 +3175,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>66</v>
       </c>
@@ -3092,7 +3189,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>66</v>
       </c>
@@ -3106,7 +3203,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>66</v>
       </c>
@@ -3120,7 +3217,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>66</v>
       </c>
@@ -3134,7 +3231,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>66</v>
       </c>
@@ -3148,7 +3245,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>66</v>
       </c>
@@ -3162,7 +3259,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>66</v>
       </c>
@@ -3176,103 +3273,103 @@
         <v>64</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="5"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="5"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
     </row>
   </sheetData>
@@ -3282,7 +3379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F5A94A-A455-4BB9-9367-9D48260B09EE}">
   <dimension ref="A1:G17"/>
   <sheetViews>
@@ -3290,9 +3387,9 @@
       <selection sqref="A1:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3313,7 +3410,7 @@
       </c>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -3332,7 +3429,7 @@
       </c>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3351,7 +3448,7 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -3370,7 +3467,7 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -3379,7 +3476,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3388,7 +3485,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3397,7 +3494,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3406,7 +3503,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -3415,7 +3512,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3424,7 +3521,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3433,7 +3530,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3442,7 +3539,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3451,7 +3548,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3460,7 +3557,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>6</v>
       </c>
@@ -3471,7 +3568,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3480,7 +3577,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>

</xml_diff>